<commit_message>
Modulos de Young Flexao
</commit_message>
<xml_diff>
--- a/Parte Experimental.xlsx
+++ b/Parte Experimental.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alves\Desktop\MCL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Farinha\Documents\GitHub\MCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9227A53E-8626-47C8-9B4B-6A47E61F6CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A01641A-E235-41B3-8307-82E2A4F8A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Medições</t>
   </si>
@@ -63,9 +62,6 @@
     <t>Deslocamento [mm]</t>
   </si>
   <si>
-    <t xml:space="preserve">Extensão </t>
-  </si>
-  <si>
     <t>Força [N]</t>
   </si>
   <si>
@@ -82,6 +78,33 @@
   </si>
   <si>
     <t>Coluna1</t>
+  </si>
+  <si>
+    <t>Tensão (Mpa)</t>
+  </si>
+  <si>
+    <t>Iy</t>
+  </si>
+  <si>
+    <t>Extensão (micro)</t>
+  </si>
+  <si>
+    <t>Carga</t>
+  </si>
+  <si>
+    <t>Descarga</t>
+  </si>
+  <si>
+    <t>Young utilizando deslocamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Média Experimental </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carga com deslocamentos </t>
+  </si>
+  <si>
+    <t>Descarga com deslocamentos</t>
   </si>
 </sst>
 </file>
@@ -258,21 +281,19 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,23 +350,60 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1161,6 +1219,551 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Carga</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$P$4:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2599999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.88E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.57E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4699999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4599999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$Q$4:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5504861982560971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1009723965121943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4267016938963399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9771878921524371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3029171895365828</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.85340338779268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.179132685176826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.504861982560969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6473-4281-ADA2-6E074AAFFFE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Descarga</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1352305429906368"/>
+                  <c:y val="0.10365266841644795"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$P$11:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.4599999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.55E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.97E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9399999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3599999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3099999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4999999999999993E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$Q$11:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15.504861982560969</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.179132685176826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.85340338779268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3029171895365828</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9771878921524371</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.4267016938963399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1009723965121943</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5504861982560971</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6473-4281-ADA2-6E074AAFFFE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1756220544"/>
+        <c:axId val="1186263888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1756220544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1186263888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1186263888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1756220544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1201,7 +1804,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1755,20 +2914,58 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2AC4F9-1F3A-4806-9F0F-6648B9F96896}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4DD7F8-7C23-4198-8BC8-ADEC6D54B33B}" name="Tabela1" displayName="Tabela1" ref="F3:J20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4DD7F8-7C23-4198-8BC8-ADEC6D54B33B}" name="Tabela1" displayName="Tabela1" ref="F3:J20" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="F3:J20" xr:uid="{DB4DD7F8-7C23-4198-8BC8-ADEC6D54B33B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3A684C29-F1BF-4452-8186-01811489FE9E}" name="Medições" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{21E60711-7A20-4B7B-9978-34C43909F7D8}" name="Força [KN]" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{22A1F2A2-0EA7-498E-B96A-F4C06FE699F1}" name="Extensão" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{910398D7-749E-4D82-B63A-2498BF78FAB1}" name="Coluna1" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{3A684C29-F1BF-4452-8186-01811489FE9E}" name="Medições" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{21E60711-7A20-4B7B-9978-34C43909F7D8}" name="Força [KN]" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{22A1F2A2-0EA7-498E-B96A-F4C06FE699F1}" name="Extensão" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{910398D7-749E-4D82-B63A-2498BF78FAB1}" name="Coluna1" dataDxfId="11">
       <calculatedColumnFormula>Tabela1[[#This Row],[Extensão]]*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{79B4D63C-04D8-49E9-A239-37B79FAEC6F8}" name="Tensão [Mpa]" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{79B4D63C-04D8-49E9-A239-37B79FAEC6F8}" name="Tensão [Mpa]" dataDxfId="10">
       <calculatedColumnFormula>Tabela1[[#This Row],[Força '[KN']]]*10^3/$C$10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1777,13 +2974,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3C16946-43BA-4D7B-A6F7-69430B072A23}" name="Tabela2" displayName="Tabela2" ref="L3:O18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="L3:O18" xr:uid="{C3C16946-43BA-4D7B-A6F7-69430B072A23}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{606B3A6A-A5F6-45A1-883D-3EACC19B9A39}" name="Medições" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C986BF1D-BE3D-499A-836E-D886A4807C16}" name="Força [N]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{0B119333-8B98-4077-A1EF-3E168290A6BE}" name="Deslocamento [mm]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{9FE34A9D-2FC7-4AEB-87BF-FBA976C43718}" name="Extensão " dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3C16946-43BA-4D7B-A6F7-69430B072A23}" name="Tabela2" displayName="Tabela2" ref="L3:R18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="L3:R18" xr:uid="{C3C16946-43BA-4D7B-A6F7-69430B072A23}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{606B3A6A-A5F6-45A1-883D-3EACC19B9A39}" name="Medições" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C986BF1D-BE3D-499A-836E-D886A4807C16}" name="Força [N]" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0B119333-8B98-4077-A1EF-3E168290A6BE}" name="Deslocamento [mm]" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9FE34A9D-2FC7-4AEB-87BF-FBA976C43718}" name="Extensão (micro)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{330B501F-A793-4B27-AF21-4D9146F4AADC}" name="Extensão" dataDxfId="1">
+      <calculatedColumnFormula>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9002FE08-366A-4DA8-A32B-4084B419B15A}" name="Tensão (Mpa)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C84BF641-AFAA-4442-801E-F8DCB2019C41}" name="Young utilizando deslocamentos" dataDxfId="0">
+      <calculatedColumnFormula>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2052,41 +3256,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O39"/>
+  <dimension ref="B2:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2106,25 +3315,34 @@
         <v>5</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>1</v>
       </c>
@@ -2163,8 +3381,20 @@
       <c r="O4" s="11">
         <v>63</v>
       </c>
+      <c r="P4" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>6.3E-5</v>
+      </c>
+      <c r="Q4" s="13">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>1.5504861982560971</v>
+      </c>
+      <c r="R4" s="13">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>21468.698779218721</v>
+      </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -2203,8 +3433,20 @@
       <c r="O5" s="11">
         <v>128</v>
       </c>
+      <c r="P5" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>1.2799999999999999E-4</v>
+      </c>
+      <c r="Q5" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>3.1009723965121943</v>
+      </c>
+      <c r="R5" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20395.263840257787</v>
+      </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>3</v>
       </c>
@@ -2243,8 +3485,20 @@
       <c r="O6" s="11">
         <v>226</v>
       </c>
+      <c r="P6" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>2.2599999999999999E-4</v>
+      </c>
+      <c r="Q6" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>5.4267016938963399</v>
+      </c>
+      <c r="R6" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20183.814356522787</v>
+      </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>4</v>
       </c>
@@ -2283,10 +3537,22 @@
       <c r="O7" s="11">
         <v>290</v>
       </c>
+      <c r="P7" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>2.9E-4</v>
+      </c>
+      <c r="Q7" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>6.9771878921524371</v>
+      </c>
+      <c r="R7" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20312.509173255636</v>
+      </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5">
         <f>AVERAGE(C4:C7)</f>
@@ -2325,10 +3591,22 @@
       <c r="O8" s="11">
         <v>388</v>
       </c>
+      <c r="P8" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>3.88E-4</v>
+      </c>
+      <c r="Q8" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>9.3029171895365828</v>
+      </c>
+      <c r="R8" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20305.019309991156</v>
+      </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4">
         <f>_xlfn.STDEV.P(C4:C7)</f>
@@ -2367,16 +3645,28 @@
       <c r="O9" s="11">
         <v>457</v>
       </c>
+      <c r="P9" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>4.57E-4</v>
+      </c>
+      <c r="Q9" s="13">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>10.85340338779268</v>
+      </c>
+      <c r="R9" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>19990.690345176823</v>
+      </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="23">
+        <v>11</v>
+      </c>
+      <c r="C10" s="20">
         <f>C8*D8</f>
         <v>257.69726249999991</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="20"/>
       <c r="F10" s="10">
         <v>7</v>
       </c>
@@ -2406,8 +3696,20 @@
       <c r="O10" s="11">
         <v>547</v>
       </c>
+      <c r="P10" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>5.4699999999999996E-4</v>
+      </c>
+      <c r="Q10" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>13.179132685176826</v>
+      </c>
+      <c r="R10" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20532.144805628643</v>
+      </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F11" s="10">
         <v>8</v>
       </c>
@@ -2437,8 +3739,27 @@
       <c r="O11" s="11">
         <v>646</v>
       </c>
+      <c r="P11" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>6.4599999999999998E-4</v>
+      </c>
+      <c r="Q11" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>15.504861982560969</v>
+      </c>
+      <c r="R11" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20388.467684362997</v>
+      </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <f>(1/12)*D8*C8^3</f>
+        <v>435.83103207242146</v>
+      </c>
       <c r="F12" s="10">
         <v>9</v>
       </c>
@@ -2468,8 +3789,20 @@
       <c r="O12" s="11">
         <v>557</v>
       </c>
+      <c r="P12" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>5.5699999999999999E-4</v>
+      </c>
+      <c r="Q12" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>13.179132685176826</v>
+      </c>
+      <c r="R12" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>19876.905328743498</v>
+      </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F13" s="10">
         <v>10</v>
       </c>
@@ -2499,8 +3832,20 @@
       <c r="O13" s="11">
         <v>455</v>
       </c>
+      <c r="P13" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>4.55E-4</v>
+      </c>
+      <c r="Q13" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>10.85340338779268</v>
+      </c>
+      <c r="R13" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>20084.433324521153</v>
+      </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F14" s="10">
         <v>11</v>
       </c>
@@ -2530,8 +3875,20 @@
       <c r="O14" s="11">
         <v>397</v>
       </c>
+      <c r="P14" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>3.97E-4</v>
+      </c>
+      <c r="Q14" s="13">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>9.3029171895365828</v>
+      </c>
+      <c r="R14" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>19408.657104131118</v>
+      </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F15" s="10">
         <v>12</v>
       </c>
@@ -2561,8 +3918,20 @@
       <c r="O15" s="11">
         <v>294</v>
       </c>
+      <c r="P15" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>2.9399999999999999E-4</v>
+      </c>
+      <c r="Q15" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>6.9771878921524371</v>
+      </c>
+      <c r="R15" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>19959.120104637925</v>
+      </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F16" s="10">
         <v>13</v>
       </c>
@@ -2592,8 +3961,20 @@
       <c r="O16" s="11">
         <v>236</v>
       </c>
+      <c r="P16" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>2.3599999999999999E-4</v>
+      </c>
+      <c r="Q16" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>5.4267016938963399</v>
+      </c>
+      <c r="R16" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>18809.861249249603</v>
+      </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F17" s="10">
         <v>14</v>
       </c>
@@ -2623,8 +4004,20 @@
       <c r="O17" s="11">
         <v>131</v>
       </c>
+      <c r="P17" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>1.3099999999999999E-4</v>
+      </c>
+      <c r="Q17" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>3.1009723965121943</v>
+      </c>
+      <c r="R17" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>19424.060800245512</v>
+      </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F18" s="10">
         <v>15</v>
       </c>
@@ -2654,8 +4047,20 @@
       <c r="O18" s="13">
         <v>75</v>
       </c>
+      <c r="P18" s="25">
+        <f>Tabela2[[#This Row],[Extensão (micro)]]*10^(-6)</f>
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="Q18" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*(200-50)*C8/(2*C12)</f>
+        <v>1.5504861982560971</v>
+      </c>
+      <c r="R18" s="23">
+        <f>Tabela2[[#This Row],[Força '[N']]]*200^3/(3*Tabela2[[#This Row],[Deslocamento '[mm']]]*$C$12)</f>
+        <v>15470.490902850406</v>
+      </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F19" s="10">
         <v>16</v>
       </c>
@@ -2678,7 +4083,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F20" s="12">
         <v>17</v>
       </c>
@@ -2697,7 +4102,18 @@
         <v>4.346185089956089</v>
       </c>
     </row>
-    <row r="39" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>17</v>
+      </c>
+      <c r="O38" t="s">
+        <v>18</v>
+      </c>
+      <c r="P38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H39">
         <v>35137</v>
       </c>
@@ -2714,13 +4130,45 @@
       <c r="L39">
         <f>(K39-J39)/K39*100</f>
         <v>12.422138513430337</v>
+      </c>
+      <c r="N39">
+        <v>23927</v>
+      </c>
+      <c r="O39">
+        <v>24183</v>
+      </c>
+      <c r="P39">
+        <f>AVERAGE(N39,O39)</f>
+        <v>24055</v>
+      </c>
+    </row>
+    <row r="41" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <f>AVERAGE(R4:R11)</f>
+        <v>20447.076036801816</v>
+      </c>
+      <c r="O42">
+        <f>AVERAGE(R11:R18)</f>
+        <v>19177.749562342775</v>
+      </c>
+      <c r="P42">
+        <f>AVERAGE(N42,O42)</f>
+        <v>19812.412799572296</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="L2:O2"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="L2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
ponto 7 alinea a
</commit_message>
<xml_diff>
--- a/Parte Experimental.xlsx
+++ b/Parte Experimental.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Farinha\Documents\GitHub\MCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC8FC9A-BB69-4626-94AA-AD38B6BAD36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F1A4FA-DC6C-426E-8E26-CB2A29AB9636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Medições</t>
   </si>
@@ -106,6 +106,18 @@
   <si>
     <t>Descarga com deslocamentos</t>
   </si>
+  <si>
+    <t xml:space="preserve">Deslocamentos (Ponto 7) </t>
+  </si>
+  <si>
+    <t>microExtensões (Ponto 7)</t>
+  </si>
+  <si>
+    <t>Desvios carga(%)</t>
+  </si>
+  <si>
+    <t>Desvios descarga(%)</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +159,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +381,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3253,10 +3277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R42"/>
+  <dimension ref="B2:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:Q18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,6 +3299,9 @@
     <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
@@ -3971,7 +3998,7 @@
         <v>18809.861249249603</v>
       </c>
     </row>
-    <row r="17" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F17" s="10">
         <v>14</v>
       </c>
@@ -4014,7 +4041,7 @@
         <v>19424.060800245512</v>
       </c>
     </row>
-    <row r="18" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F18" s="10">
         <v>15</v>
       </c>
@@ -4057,7 +4084,7 @@
         <v>15470.490902850406</v>
       </c>
     </row>
-    <row r="19" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F19" s="10">
         <v>16</v>
       </c>
@@ -4080,7 +4107,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F20" s="12">
         <v>17</v>
       </c>
@@ -4097,6 +4124,186 @@
       <c r="J20" s="18">
         <f>Tabela1[[#This Row],[Força '[KN']]]*10^3/$C$10</f>
         <v>4.346185089956089</v>
+      </c>
+      <c r="S20" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" t="s">
+        <v>24</v>
+      </c>
+      <c r="U20" t="s">
+        <v>25</v>
+      </c>
+      <c r="V20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R21" s="25">
+        <v>2</v>
+      </c>
+      <c r="S21">
+        <f>R21*200^(3)/(3*$P$39*$C$12)</f>
+        <v>0.50871578899000924</v>
+      </c>
+      <c r="T21">
+        <f>(Q4/$P$39)*10^6</f>
+        <v>64.455880201874749</v>
+      </c>
+      <c r="U21">
+        <f>ABS(T21-O4)/T21*100</f>
+        <v>2.2587236374942918</v>
+      </c>
+      <c r="V21">
+        <f>ABS(T21-O18)/T21*100</f>
+        <v>16.358662336316318</v>
+      </c>
+    </row>
+    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R22" s="26">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <f t="shared" ref="S22:S28" si="0">R22*200^(3)/(3*$P$39*$C$12)</f>
+        <v>1.0174315779800185</v>
+      </c>
+      <c r="T22">
+        <f t="shared" ref="T22:T28" si="1">(Q5/$P$39)*10^6</f>
+        <v>128.9117604037495</v>
+      </c>
+      <c r="U22">
+        <f t="shared" ref="U22:U28" si="2">ABS(T22-O5)/T22*100</f>
+        <v>0.70727480634340778</v>
+      </c>
+      <c r="V22">
+        <f>ABS(T22-O17)/T22*100</f>
+        <v>1.6198984403829184</v>
+      </c>
+    </row>
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R23" s="25">
+        <v>7</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="0"/>
+        <v>1.7805052614650323</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>225.59558070656163</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="2"/>
+        <v>0.17926738288566263</v>
+      </c>
+      <c r="V23">
+        <f>ABS(T23-O16)/T23*100</f>
+        <v>4.6119783290310457</v>
+      </c>
+    </row>
+    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R24" s="26">
+        <v>9</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="0"/>
+        <v>2.2892210504550414</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>290.05146090843635</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="2"/>
+        <v>1.7741992498565423E-2</v>
+      </c>
+      <c r="V24">
+        <f>ABS(T24-O15)/T24*100</f>
+        <v>1.3613236351911095</v>
+      </c>
+    </row>
+    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R25" s="25">
+        <v>12</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="0"/>
+        <v>3.0522947339400552</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>386.73528121124849</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="2"/>
+        <v>0.32702441442384839</v>
+      </c>
+      <c r="V25">
+        <f>ABS(T25-O14)/T25*100</f>
+        <v>2.6541976611501745</v>
+      </c>
+    </row>
+    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R26" s="26">
+        <v>14</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>3.5610105229300646</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>451.19116141312327</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="2"/>
+        <v>1.2874451194220085</v>
+      </c>
+      <c r="V26">
+        <f>ABS(T26-O13)/T26*100</f>
+        <v>0.84417402480747006</v>
+      </c>
+    </row>
+    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R27" s="25">
+        <v>17</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="0"/>
+        <v>4.324084206415078</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>547.87498171593541</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="2"/>
+        <v>0.15970463064310345</v>
+      </c>
+      <c r="V27">
+        <f>ABS(T27-O12)/T27*100</f>
+        <v>1.6655292883579369</v>
+      </c>
+    </row>
+    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="R28" s="26">
+        <v>20</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="0"/>
+        <v>5.0871578899000918</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>644.55880201874743</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="2"/>
+        <v>0.22359449234713161</v>
+      </c>
+      <c r="V28">
+        <f>ABS(T28-O11)/T28*100</f>
+        <v>0.22359449234713161</v>
       </c>
     </row>
     <row r="38" spans="8:16" x14ac:dyDescent="0.25">

</xml_diff>